<commit_message>
17/10/18 David --> Introducción + estudio mercado + analisis de competencia + cronograma + sistema de JSON + test temporal + Expandable List View
</commit_message>
<xml_diff>
--- a/documentacion/Cronología.xlsx
+++ b/documentacion/Cronología.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\android\documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>OCTUBRE</t>
   </si>
@@ -51,9 +51,6 @@
     <t>ENERO</t>
   </si>
   <si>
-    <t>No realizado</t>
-  </si>
-  <si>
     <t>Cronología + Estimación de horas</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Control de versiones Git + readme.md</t>
   </si>
   <si>
-    <t>26/06/17 No efectuado por el momento</t>
-  </si>
-  <si>
     <t>Creando iconos normal y redondeado</t>
   </si>
   <si>
@@ -115,12 +109,45 @@
   </si>
   <si>
     <t>Realizado el 07/10/18</t>
+  </si>
+  <si>
+    <t>Clases "Reuniones"</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Crear JSON Files + Funciones que los recorran</t>
+  </si>
+  <si>
+    <t>Crear Expandable ListView</t>
+  </si>
+  <si>
+    <t>Realizado el 13/10/18</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Documentación código fuente</t>
+  </si>
+  <si>
+    <t>Back up's Git</t>
+  </si>
+  <si>
+    <t>Realizado el 10/10/18</t>
+  </si>
+  <si>
+    <t>Expandable subitem clic go to test</t>
+  </si>
+  <si>
+    <t>26/06/17 Suspendido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -145,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,13 +193,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -354,22 +387,43 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -380,27 +434,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -416,6 +449,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -423,6 +468,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -513,7 +570,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -548,7 +605,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -725,7 +782,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -735,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,109 +824,109 @@
       <c r="M1" s="2"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="21"/>
-      <c r="AA4" s="22"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="19"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="24"/>
-      <c r="AA5" s="25"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="22"/>
     </row>
     <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="22"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
       <c r="J6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="16" t="s">
+      <c r="K6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="16" t="s">
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="16" t="s">
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="18"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="25"/>
       <c r="AA6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="AB6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC6" s="17"/>
-      <c r="AD6" s="18"/>
+      <c r="AB6" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="25"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B7" s="28"/>
@@ -933,17 +990,17 @@
       </c>
       <c r="AA7" s="27"/>
       <c r="AB7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AC7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD7" s="11" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
+      <c r="B8" s="12">
         <v>1</v>
       </c>
       <c r="C8" s="31" t="s">
@@ -955,32 +1012,32 @@
       <c r="G8" s="32"/>
       <c r="H8" s="32"/>
       <c r="I8" s="33"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="4">
+      <c r="J8" s="13"/>
+      <c r="K8" s="12">
         <v>5</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-      <c r="AA8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB8" s="4">
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB8" s="12">
         <v>5</v>
       </c>
-      <c r="AC8" s="4">
+      <c r="AC8" s="12">
         <f>SUM(J8:Z8)</f>
         <v>5</v>
       </c>
@@ -990,11 +1047,11 @@
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
+      <c r="B9" s="12">
         <v>2</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="32"/>
@@ -1002,32 +1059,32 @@
       <c r="G9" s="32"/>
       <c r="H9" s="32"/>
       <c r="I9" s="33"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4">
+      <c r="J9" s="12"/>
+      <c r="K9" s="12">
         <v>7</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB9" s="4">
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB9" s="12">
         <v>10</v>
       </c>
-      <c r="AC9" s="4">
+      <c r="AC9" s="12">
         <f t="shared" ref="AC9:AC27" si="0">SUM(J9:Z9)</f>
         <v>7</v>
       </c>
@@ -1037,91 +1094,91 @@
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
+      <c r="B10" s="14">
         <v>3</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="12">
-        <v>20</v>
-      </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB10" s="4">
+      <c r="C10" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="14">
+        <v>30</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB10" s="14">
         <v>10</v>
       </c>
-      <c r="AC10" s="4">
+      <c r="AC10" s="14">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="AD10" s="4">
         <f t="shared" si="1"/>
-        <v>-10</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
+      <c r="B11" s="12">
         <v>4</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="4">
+      <c r="C11" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="12">
         <v>10</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
-      <c r="AA11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB11" s="4">
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB11" s="12">
         <v>10</v>
       </c>
-      <c r="AC11" s="4">
+      <c r="AC11" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1131,44 +1188,44 @@
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B12" s="4">
+      <c r="B12" s="12">
         <v>5</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="12">
+        <v>10</v>
+      </c>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="4">
-        <v>10</v>
-      </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB12" s="4">
+      <c r="AB12" s="12">
         <v>8</v>
       </c>
-      <c r="AC12" s="4">
+      <c r="AC12" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1178,44 +1235,44 @@
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
+      <c r="B13" s="12">
         <v>6</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="4">
+      <c r="C13" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="12">
         <v>1.5</v>
       </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB13" s="4">
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB13" s="12">
         <v>2.5</v>
       </c>
-      <c r="AC13" s="4">
+      <c r="AC13" s="12">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
@@ -1225,44 +1282,44 @@
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
+      <c r="B14" s="12">
         <v>7</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="4">
+      <c r="C14" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="12">
         <v>3</v>
       </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB14" s="4">
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
+      <c r="AA14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB14" s="12">
         <v>5</v>
       </c>
-      <c r="AC14" s="4">
+      <c r="AC14" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1272,44 +1329,44 @@
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
+      <c r="B15" s="12">
         <v>8</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12"/>
+      <c r="AA15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB15" s="4">
+      <c r="AB15" s="12">
         <v>3</v>
       </c>
-      <c r="AC15" s="4">
+      <c r="AC15" s="12">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
@@ -1319,44 +1376,44 @@
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
+      <c r="B16" s="12">
         <v>9</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12">
+        <v>9</v>
+      </c>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4">
-        <v>9</v>
-      </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB16" s="4">
+      <c r="AB16" s="12">
         <v>10</v>
       </c>
-      <c r="AC16" s="4">
+      <c r="AC16" s="12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1366,44 +1423,44 @@
       </c>
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B17" s="4">
+      <c r="B17" s="12">
         <v>10</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4">
+      <c r="C17" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12">
         <v>7.5</v>
       </c>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB17" s="4">
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB17" s="12">
         <v>10</v>
       </c>
-      <c r="AC17" s="4">
+      <c r="AC17" s="12">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
@@ -1413,136 +1470,166 @@
       </c>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B18" s="4">
+      <c r="B18" s="12">
         <v>11</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="4"/>
-      <c r="AC18" s="4">
+      <c r="C18" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="L18" s="12">
+        <v>16</v>
+      </c>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
+      <c r="AA18" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB18" s="12">
+        <v>20</v>
+      </c>
+      <c r="AC18" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16.5</v>
       </c>
       <c r="AD18" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
+      <c r="B19" s="12">
         <v>12</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
-      <c r="AA19" s="3"/>
-      <c r="AB19" s="4"/>
-      <c r="AC19" s="4">
+      <c r="C19" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="12">
+        <v>2</v>
+      </c>
+      <c r="K19" s="12">
+        <v>2</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="12"/>
+      <c r="AC19" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AD19" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="20" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
+      <c r="B20" s="12">
         <v>13</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="4"/>
-      <c r="AC20" s="4">
+      <c r="C20" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12">
+        <v>11</v>
+      </c>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="12"/>
+      <c r="AA20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB20" s="12">
+        <v>12</v>
+      </c>
+      <c r="AC20" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AD20" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <v>14</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
+      <c r="C21" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="37"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
+      <c r="L21" s="4">
+        <v>8</v>
+      </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -1558,30 +1645,40 @@
       <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="3"/>
-      <c r="AB21" s="4"/>
+      <c r="AB21" s="4">
+        <v>50</v>
+      </c>
       <c r="AC21" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD21" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <v>15</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
+      <c r="C22" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0.5</v>
+      </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
@@ -1597,31 +1694,43 @@
       <c r="Y22" s="4"/>
       <c r="Z22" s="4"/>
       <c r="AA22" s="3"/>
-      <c r="AB22" s="4"/>
+      <c r="AB22" s="4">
+        <v>6.5</v>
+      </c>
       <c r="AC22" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AD22" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>16</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
+      <c r="C23" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="4">
+        <v>20</v>
+      </c>
+      <c r="K23" s="4">
+        <v>8</v>
+      </c>
+      <c r="L23" s="4">
+        <v>6</v>
+      </c>
+      <c r="M23" s="4">
+        <v>6</v>
+      </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
@@ -1636,27 +1745,29 @@
       <c r="Y23" s="4"/>
       <c r="Z23" s="4"/>
       <c r="AA23" s="3"/>
-      <c r="AB23" s="4"/>
+      <c r="AB23" s="4">
+        <v>50</v>
+      </c>
       <c r="AC23" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AD23" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>17</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -1689,13 +1800,13 @@
       <c r="B25" s="4">
         <v>18</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
@@ -1728,13 +1839,13 @@
       <c r="B26" s="4">
         <v>19</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
@@ -1767,13 +1878,13 @@
       <c r="B27" s="4">
         <v>20</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -1805,19 +1916,19 @@
     <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="J28">
         <f>SUM(J8:J27)</f>
-        <v>44.5</v>
+        <v>77</v>
       </c>
       <c r="K28">
         <f>SUM(K8:K27)</f>
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="L28">
         <f t="shared" ref="L28:Z28" si="2">SUM(L8:L27)</f>
-        <v>0</v>
+        <v>41.5</v>
       </c>
       <c r="M28">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N28">
         <f t="shared" si="2"/>
@@ -1871,45 +1982,63 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB28" s="13">
+      <c r="AB28" s="10">
         <f>SUM(AB8:AB27)</f>
-        <v>73.5</v>
-      </c>
-      <c r="AC28" s="13">
+        <v>212</v>
+      </c>
+      <c r="AC28" s="10">
         <f>SUM(AC8:AC27)</f>
-        <v>75.5</v>
+        <v>166.5</v>
       </c>
       <c r="AD28" s="4">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="29" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="C29" s="14"/>
-      <c r="E29" s="15" t="s">
+      <c r="C29" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="2"/>
       <c r="H29" s="1"/>
-      <c r="J29" s="3"/>
-      <c r="L29" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="P29" s="10"/>
-      <c r="R29" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
-      <c r="U29" s="15"/>
-      <c r="V29" s="15"/>
-      <c r="W29" s="15"/>
+      <c r="I29" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+      <c r="R29" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="S29" s="40"/>
+      <c r="T29" s="40"/>
+      <c r="U29" s="40"/>
+      <c r="V29" s="40"/>
+      <c r="W29" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="I29:N29"/>
+    <mergeCell ref="R29:W29"/>
+    <mergeCell ref="AB6:AD6"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="C17:I17"/>
+    <mergeCell ref="C24:I24"/>
     <mergeCell ref="C25:I25"/>
     <mergeCell ref="C26:I26"/>
     <mergeCell ref="C27:I27"/>
@@ -1925,31 +2054,8 @@
     <mergeCell ref="C8:I8"/>
     <mergeCell ref="C9:I9"/>
     <mergeCell ref="C23:I23"/>
-    <mergeCell ref="R29:W29"/>
-    <mergeCell ref="AB6:AD6"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="C15:I15"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="C17:I17"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="C24:I24"/>
   </mergeCells>
   <conditionalFormatting sqref="AD8:AD28">
-    <cfRule type="iconSet" priority="3">
-      <iconSet iconSet="3Flags">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0"/>
-      </iconSet>
-    </cfRule>
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1960,6 +2066,13 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Flags">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0"/>
+      </iconSet>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
21/10/18 David --> Verificando si el test existe y enviando un parámetro de una vista a otra
</commit_message>
<xml_diff>
--- a/documentacion/Cronología.xlsx
+++ b/documentacion/Cronología.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\android\documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>OCTUBRE</t>
   </si>
@@ -142,12 +137,21 @@
   </si>
   <si>
     <t>26/06/17 Suspendido</t>
+  </si>
+  <si>
+    <t>Realizado el 17/10/18</t>
+  </si>
+  <si>
+    <t>SharedPreferences para el JSON desde el ExpandableListView</t>
+  </si>
+  <si>
+    <t>Create function: check if exit json. If not exit show message</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,6 +408,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -425,15 +471,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -448,39 +485,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -570,7 +574,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -605,7 +609,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -782,7 +786,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -793,7 +797,7 @@
   <dimension ref="A1:AD29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,119 +828,119 @@
       <c r="M1" s="2"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
-      <c r="Z4" s="18"/>
-      <c r="AA4" s="19"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="32"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
+      <c r="AA4" s="33"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="22"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="35"/>
+      <c r="Y5" s="35"/>
+      <c r="Z5" s="35"/>
+      <c r="AA5" s="36"/>
     </row>
     <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="33"/>
       <c r="J6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="23" t="s">
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="23" t="s">
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="23" t="s">
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="26" t="s">
+      <c r="X6" s="20"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="AB6" s="23" t="s">
+      <c r="AB6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="25"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="21"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="30"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="5">
         <v>4</v>
       </c>
@@ -988,7 +992,7 @@
       <c r="Z7" s="8">
         <v>4</v>
       </c>
-      <c r="AA7" s="27"/>
+      <c r="AA7" s="38"/>
       <c r="AB7" s="6" t="s">
         <v>15</v>
       </c>
@@ -1003,15 +1007,15 @@
       <c r="B8" s="12">
         <v>1</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="33"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="26"/>
       <c r="J8" s="13"/>
       <c r="K8" s="12">
         <v>5</v>
@@ -1050,15 +1054,15 @@
       <c r="B9" s="12">
         <v>2</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="33"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="26"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12">
         <v>7</v>
@@ -1097,15 +1101,15 @@
       <c r="B10" s="14">
         <v>3</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
       <c r="J10" s="14">
         <v>30</v>
       </c>
@@ -1144,15 +1148,15 @@
       <c r="B11" s="12">
         <v>4</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
       <c r="J11" s="12">
         <v>10</v>
       </c>
@@ -1191,15 +1195,15 @@
       <c r="B12" s="12">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
       <c r="J12" s="12">
         <v>10</v>
       </c>
@@ -1238,15 +1242,15 @@
       <c r="B13" s="12">
         <v>6</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
       <c r="J13" s="12">
         <v>1.5</v>
       </c>
@@ -1285,15 +1289,15 @@
       <c r="B14" s="12">
         <v>7</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
       <c r="J14" s="12">
         <v>3</v>
       </c>
@@ -1332,15 +1336,15 @@
       <c r="B15" s="12">
         <v>8</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12">
         <v>2.5</v>
@@ -1379,15 +1383,15 @@
       <c r="B16" s="12">
         <v>9</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12">
         <v>9</v>
@@ -1426,15 +1430,15 @@
       <c r="B17" s="12">
         <v>10</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12">
         <v>7.5</v>
@@ -1473,15 +1477,15 @@
       <c r="B18" s="12">
         <v>11</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="26"/>
       <c r="J18" s="12"/>
       <c r="K18" s="12">
         <v>0.5</v>
@@ -1522,15 +1526,15 @@
       <c r="B19" s="12">
         <v>12</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
       <c r="J19" s="12">
         <v>2</v>
       </c>
@@ -1569,15 +1573,15 @@
       <c r="B20" s="12">
         <v>13</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12">
@@ -1613,63 +1617,67 @@
       </c>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B21" s="4">
+      <c r="B21" s="12">
         <v>14</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4">
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12">
         <v>8</v>
       </c>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="3"/>
-      <c r="AB21" s="4">
-        <v>50</v>
-      </c>
-      <c r="AC21" s="4">
+      <c r="M21" s="12">
+        <v>4</v>
+      </c>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12"/>
+      <c r="AA21" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB21" s="12">
+        <v>20</v>
+      </c>
+      <c r="AC21" s="12">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="AD21" s="4">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <v>15</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="29"/>
       <c r="J22" s="4">
         <v>0.5</v>
       </c>
@@ -1679,7 +1687,9 @@
       <c r="L22" s="4">
         <v>0.5</v>
       </c>
-      <c r="M22" s="4"/>
+      <c r="M22" s="4">
+        <v>0.5</v>
+      </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -1699,37 +1709,37 @@
       </c>
       <c r="AC22" s="4">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AD22" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>16</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="4">
-        <v>20</v>
-      </c>
-      <c r="K23" s="4">
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="12">
+        <v>16</v>
+      </c>
+      <c r="K23" s="12">
         <v>8</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="12">
         <v>6</v>
       </c>
-      <c r="M23" s="4">
-        <v>6</v>
+      <c r="M23" s="12">
+        <v>12</v>
       </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
@@ -1746,32 +1756,36 @@
       <c r="Z23" s="4"/>
       <c r="AA23" s="3"/>
       <c r="AB23" s="4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AC23" s="4">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AD23" s="4">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>17</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
+      <c r="C24" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
+      <c r="M24" s="12">
+        <v>6</v>
+      </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
@@ -1786,49 +1800,57 @@
       <c r="Y24" s="4"/>
       <c r="Z24" s="4"/>
       <c r="AA24" s="3"/>
-      <c r="AB24" s="4"/>
+      <c r="AB24" s="4">
+        <v>10</v>
+      </c>
       <c r="AC24" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AD24" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
+      <c r="B25" s="12">
         <v>18</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
-      <c r="AA25" s="3"/>
-      <c r="AB25" s="4"/>
-      <c r="AC25" s="4">
+      <c r="C25" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12">
+        <v>6</v>
+      </c>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="12"/>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="12">
+        <v>6</v>
+      </c>
+      <c r="AC25" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AD25" s="4">
         <f t="shared" si="1"/>
@@ -1839,13 +1861,13 @@
       <c r="B26" s="4">
         <v>19</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
@@ -1878,13 +1900,13 @@
       <c r="B27" s="4">
         <v>20</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -1916,7 +1938,7 @@
     <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="J28">
         <f>SUM(J8:J27)</f>
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K28">
         <f>SUM(K8:K27)</f>
@@ -1928,7 +1950,7 @@
       </c>
       <c r="M28">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>28.5</v>
       </c>
       <c r="N28">
         <f t="shared" si="2"/>
@@ -1984,45 +2006,60 @@
       </c>
       <c r="AB28" s="10">
         <f>SUM(AB8:AB27)</f>
-        <v>212</v>
+        <v>248</v>
       </c>
       <c r="AC28" s="10">
         <f>SUM(AC8:AC27)</f>
-        <v>166.5</v>
+        <v>185</v>
       </c>
       <c r="AD28" s="4">
         <f t="shared" si="1"/>
-        <v>45.5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
       <c r="G29" s="2"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="39" t="s">
+      <c r="I29" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="R29" s="40" t="s">
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="R29" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="S29" s="40"/>
-      <c r="T29" s="40"/>
-      <c r="U29" s="40"/>
-      <c r="V29" s="40"/>
-      <c r="W29" s="40"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="18"/>
+      <c r="W29" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="B4:AA5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="S6:V6"/>
+    <mergeCell ref="W6:Z6"/>
+    <mergeCell ref="AA6:AA7"/>
+    <mergeCell ref="B6:I7"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C23:I23"/>
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="I29:N29"/>
     <mergeCell ref="R29:W29"/>
@@ -2039,21 +2076,6 @@
     <mergeCell ref="C16:I16"/>
     <mergeCell ref="C17:I17"/>
     <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="B4:AA5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="S6:V6"/>
-    <mergeCell ref="W6:Z6"/>
-    <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="B6:I7"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="C19:I19"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C23:I23"/>
   </mergeCells>
   <conditionalFormatting sqref="AD8:AD28">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
12/11/18 David --> Mejorando nota final, añadiendo colores a los clicks de las respuestas, evitando el retroceso en el test o pdf
</commit_message>
<xml_diff>
--- a/documentacion/Cronología.xlsx
+++ b/documentacion/Cronología.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>OCTUBRE</t>
   </si>
@@ -146,6 +146,30 @@
   </si>
   <si>
     <t>Create function: check if exit json. If not exit show message</t>
+  </si>
+  <si>
+    <t>Deshabilitar botón next y mostrar botón finish al acabar el JSON</t>
+  </si>
+  <si>
+    <t>Una vez salgas del test a layout nota no back to test otra vez</t>
+  </si>
+  <si>
+    <t>Vista sistema puntuación test + calculo nota final</t>
+  </si>
+  <si>
+    <t>Realizado el 20/10/18</t>
+  </si>
+  <si>
+    <t>Realizado el 22/10/18</t>
+  </si>
+  <si>
+    <t>Realizado el 30/10/18</t>
+  </si>
+  <si>
+    <t>Realizado el 01/11/18</t>
+  </si>
+  <si>
+    <t>Realizado el 02/11/18</t>
   </si>
 </sst>
 </file>
@@ -369,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -408,6 +432,72 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -417,74 +507,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,18 +827,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD29"/>
+  <dimension ref="A1:AD33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" customWidth="1"/>
-    <col min="4" max="9" width="7.28515625" customWidth="1"/>
+    <col min="2" max="9" width="7.140625" customWidth="1"/>
     <col min="10" max="26" width="4.7109375" customWidth="1"/>
     <col min="27" max="27" width="28.7109375" customWidth="1"/>
     <col min="28" max="30" width="11.7109375" customWidth="1"/>
@@ -828,119 +859,119 @@
       <c r="M1" s="2"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="32"/>
-      <c r="AA4" s="33"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="23"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="35"/>
-      <c r="AA5" s="36"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="26"/>
     </row>
     <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="33"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="23"/>
       <c r="J6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="19" t="s">
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="19" t="s">
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="T6" s="20"/>
-      <c r="U6" s="20"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="19" t="s">
+      <c r="T6" s="28"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="X6" s="20"/>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="21"/>
-      <c r="AA6" s="37" t="s">
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="AB6" s="19" t="s">
+      <c r="AB6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="AC6" s="20"/>
-      <c r="AD6" s="21"/>
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="29"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="41"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="5">
         <v>4</v>
       </c>
@@ -992,7 +1023,7 @@
       <c r="Z7" s="8">
         <v>4</v>
       </c>
-      <c r="AA7" s="38"/>
+      <c r="AA7" s="31"/>
       <c r="AB7" s="6" t="s">
         <v>15</v>
       </c>
@@ -1007,15 +1038,15 @@
       <c r="B8" s="12">
         <v>1</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="26"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="13"/>
       <c r="K8" s="12">
         <v>5</v>
@@ -1054,15 +1085,15 @@
       <c r="B9" s="12">
         <v>2</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="37"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12">
         <v>7</v>
@@ -1093,7 +1124,7 @@
         <v>7</v>
       </c>
       <c r="AD9" s="4">
-        <f t="shared" ref="AD9:AD28" si="1">AB9-AC9</f>
+        <f t="shared" ref="AD9:AD32" si="1">AB9-AC9</f>
         <v>3</v>
       </c>
     </row>
@@ -1101,15 +1132,15 @@
       <c r="B10" s="14">
         <v>3</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="14">
         <v>30</v>
       </c>
@@ -1148,15 +1179,15 @@
       <c r="B11" s="12">
         <v>4</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
       <c r="J11" s="12">
         <v>10</v>
       </c>
@@ -1195,15 +1226,15 @@
       <c r="B12" s="12">
         <v>5</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="12">
         <v>10</v>
       </c>
@@ -1242,15 +1273,15 @@
       <c r="B13" s="12">
         <v>6</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
       <c r="J13" s="12">
         <v>1.5</v>
       </c>
@@ -1289,15 +1320,15 @@
       <c r="B14" s="12">
         <v>7</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
       <c r="J14" s="12">
         <v>3</v>
       </c>
@@ -1336,15 +1367,15 @@
       <c r="B15" s="12">
         <v>8</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12">
         <v>2.5</v>
@@ -1383,15 +1414,15 @@
       <c r="B16" s="12">
         <v>9</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12">
         <v>9</v>
@@ -1430,15 +1461,15 @@
       <c r="B17" s="12">
         <v>10</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12">
         <v>7.5</v>
@@ -1477,15 +1508,15 @@
       <c r="B18" s="12">
         <v>11</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="26"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="12"/>
       <c r="K18" s="12">
         <v>0.5</v>
@@ -1526,28 +1557,36 @@
       <c r="B19" s="12">
         <v>12</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
       <c r="J19" s="12">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K19" s="12">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="L19" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
+      <c r="M19" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="N19" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P19" s="12">
+        <v>1.5</v>
+      </c>
       <c r="Q19" s="12"/>
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
@@ -1562,26 +1601,26 @@
       <c r="AB19" s="12"/>
       <c r="AC19" s="12">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="AD19" s="4">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>-7.5</v>
       </c>
     </row>
     <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B20" s="12">
         <v>13</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12">
@@ -1620,15 +1659,15 @@
       <c r="B21" s="12">
         <v>14</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="26"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="37"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12">
@@ -1669,15 +1708,15 @@
       <c r="B22" s="4">
         <v>15</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="29"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="19"/>
       <c r="J22" s="4">
         <v>0.5</v>
       </c>
@@ -1690,9 +1729,15 @@
       <c r="M22" s="4">
         <v>0.5</v>
       </c>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
+      <c r="N22" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O22" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="P22" s="4">
+        <v>0.5</v>
+      </c>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
@@ -1709,26 +1754,26 @@
       </c>
       <c r="AC22" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="AD22" s="4">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>16</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="29"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="19"/>
       <c r="J23" s="12">
         <v>16</v>
       </c>
@@ -1743,7 +1788,9 @@
       </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
+      <c r="P23" s="4">
+        <v>3</v>
+      </c>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
@@ -1760,50 +1807,52 @@
       </c>
       <c r="AC23" s="4">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="AD23" s="4">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B24" s="4">
+      <c r="B24" s="12">
         <v>17</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
       <c r="M24" s="12">
         <v>6</v>
       </c>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
-      <c r="Z24" s="4"/>
-      <c r="AA24" s="3"/>
-      <c r="AB24" s="4">
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12"/>
+      <c r="W24" s="12"/>
+      <c r="X24" s="12"/>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="12"/>
+      <c r="AA24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB24" s="12">
         <v>10</v>
       </c>
-      <c r="AC24" s="4">
+      <c r="AC24" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1816,15 +1865,15 @@
       <c r="B25" s="12">
         <v>18</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
@@ -1844,7 +1893,9 @@
       <c r="X25" s="12"/>
       <c r="Y25" s="12"/>
       <c r="Z25" s="12"/>
-      <c r="AA25" s="11"/>
+      <c r="AA25" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="AB25" s="12">
         <v>6</v>
       </c>
@@ -1858,38 +1909,48 @@
       </c>
     </row>
     <row r="26" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
+      <c r="B26" s="12">
         <v>19</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
-      <c r="AA26" s="3"/>
-      <c r="AB26" s="4"/>
-      <c r="AC26" s="4">
+      <c r="C26" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12">
+        <v>15</v>
+      </c>
+      <c r="O26" s="12">
+        <v>3</v>
+      </c>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB26" s="12">
+        <v>18</v>
+      </c>
+      <c r="AC26" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AD26" s="4">
         <f t="shared" si="1"/>
@@ -1897,172 +1958,324 @@
       </c>
     </row>
     <row r="27" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B27" s="4">
+      <c r="B27" s="12">
         <v>20</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
-      <c r="AA27" s="3"/>
-      <c r="AB27" s="4"/>
-      <c r="AC27" s="4">
+      <c r="C27" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12">
+        <v>8</v>
+      </c>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB27" s="12">
+        <v>10</v>
+      </c>
+      <c r="AC27" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD27" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="J28">
-        <f>SUM(J8:J27)</f>
-        <v>73</v>
-      </c>
-      <c r="K28">
-        <f>SUM(K8:K27)</f>
-        <v>42</v>
-      </c>
-      <c r="L28">
-        <f t="shared" ref="L28:Z28" si="2">SUM(L8:L27)</f>
-        <v>41.5</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="2"/>
-        <v>28.5</v>
-      </c>
-      <c r="N28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="V28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="W28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="X28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Y28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AB28" s="10">
-        <f>SUM(AB8:AB27)</f>
-        <v>248</v>
-      </c>
-      <c r="AC28" s="10">
-        <f>SUM(AC8:AC27)</f>
-        <v>185</v>
+      <c r="B28" s="12">
+        <v>21</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12">
+        <v>3</v>
+      </c>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12"/>
+      <c r="AA28" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB28" s="12">
+        <v>5</v>
+      </c>
+      <c r="AC28" s="12">
+        <v>3</v>
       </c>
       <c r="AD28" s="4">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="C29" s="16" t="s">
+      <c r="B29" s="4">
+        <v>22</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>23</v>
+      </c>
+      <c r="C30" s="42"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <v>24</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="4">
+        <v>10</v>
+      </c>
+      <c r="AC31" s="4">
+        <f t="shared" ref="AC31" si="2">SUM(J31:Z31)</f>
+        <v>0</v>
+      </c>
+      <c r="AD31" s="4">
+        <f t="shared" ref="AD31" si="3">AB31-AC31</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <f>SUM(J8:J31)</f>
+        <v>72.5</v>
+      </c>
+      <c r="K32">
+        <f t="shared" ref="K32:Z32" si="4">SUM(K8:K31)</f>
+        <v>41.5</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="4"/>
+        <v>41.5</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="4"/>
+        <v>6.5</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AB32" s="10">
+        <f>SUM(AB8:AB27)</f>
+        <v>276</v>
+      </c>
+      <c r="AC32" s="10">
+        <f>SUM(AC8:AC27)</f>
+        <v>219</v>
+      </c>
+      <c r="AD32" s="4">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C33" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="17" t="s">
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="R29" s="18" t="s">
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="39"/>
+      <c r="R33" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="S29" s="18"/>
-      <c r="T29" s="18"/>
-      <c r="U29" s="18"/>
-      <c r="V29" s="18"/>
-      <c r="W29" s="18"/>
+      <c r="S33" s="40"/>
+      <c r="T33" s="40"/>
+      <c r="U33" s="40"/>
+      <c r="V33" s="40"/>
+      <c r="W33" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="B4:AA5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="S6:V6"/>
-    <mergeCell ref="W6:Z6"/>
-    <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="B6:I7"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="C19:I19"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="I29:N29"/>
-    <mergeCell ref="R29:W29"/>
+  <mergeCells count="35">
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="I33:N33"/>
+    <mergeCell ref="R33:W33"/>
     <mergeCell ref="AB6:AD6"/>
     <mergeCell ref="C10:I10"/>
     <mergeCell ref="C11:I11"/>
@@ -2076,8 +2289,46 @@
     <mergeCell ref="C16:I16"/>
     <mergeCell ref="C17:I17"/>
     <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="B4:AA5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="S6:V6"/>
+    <mergeCell ref="W6:Z6"/>
+    <mergeCell ref="AA6:AA7"/>
+    <mergeCell ref="B6:I7"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C30:I30"/>
   </mergeCells>
-  <conditionalFormatting sqref="AD8:AD28">
+  <conditionalFormatting sqref="AD8:AD30 AD32">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="iconSet" priority="5">
+      <iconSet iconSet="3Flags">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD31">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2088,7 +2339,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="iconSet" priority="3">
+    <cfRule type="iconSet" priority="2">
       <iconSet iconSet="3Flags">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
30/11/18 David --> Creo la BBDD y compruebo que se guardan bien los resultados, falta mostrar el resultado en la sección de resultados
</commit_message>
<xml_diff>
--- a/documentacion/Cronología.xlsx
+++ b/documentacion/Cronología.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>OCTUBRE</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>Realizado el 02/11/18</t>
+  </si>
+  <si>
+    <t>Realizar BBDD + inserts</t>
+  </si>
+  <si>
+    <t>Listview resultados</t>
+  </si>
+  <si>
+    <t>Realizado el 14/11/18</t>
   </si>
 </sst>
 </file>
@@ -393,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -444,6 +453,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -489,15 +507,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -509,15 +518,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,7 +830,7 @@
   <dimension ref="A1:AD33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AA29" sqref="AA29"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,119 +859,119 @@
       <c r="M1" s="2"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="23"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="26"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B5" s="24"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="25"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="29"/>
     </row>
     <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="23"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
       <c r="J6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="27" t="s">
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="27" t="s">
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="T6" s="28"/>
-      <c r="U6" s="28"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="27" t="s">
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="32"/>
+      <c r="W6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="28"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="30" t="s">
+      <c r="X6" s="31"/>
+      <c r="Y6" s="31"/>
+      <c r="Z6" s="32"/>
+      <c r="AA6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="AB6" s="27" t="s">
+      <c r="AB6" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="AC6" s="28"/>
-      <c r="AD6" s="29"/>
+      <c r="AC6" s="31"/>
+      <c r="AD6" s="32"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="5">
         <v>4</v>
       </c>
@@ -1023,7 +1023,7 @@
       <c r="Z7" s="8">
         <v>4</v>
       </c>
-      <c r="AA7" s="31"/>
+      <c r="AA7" s="34"/>
       <c r="AB7" s="6" t="s">
         <v>15</v>
       </c>
@@ -1038,15 +1038,15 @@
       <c r="B8" s="12">
         <v>1</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="37"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="22"/>
       <c r="J8" s="13"/>
       <c r="K8" s="12">
         <v>5</v>
@@ -1085,15 +1085,15 @@
       <c r="B9" s="12">
         <v>2</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12">
         <v>7</v>
@@ -1179,15 +1179,15 @@
       <c r="B11" s="12">
         <v>4</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
       <c r="J11" s="12">
         <v>10</v>
       </c>
@@ -1226,15 +1226,15 @@
       <c r="B12" s="12">
         <v>5</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
       <c r="J12" s="12">
         <v>10</v>
       </c>
@@ -1273,15 +1273,15 @@
       <c r="B13" s="12">
         <v>6</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
       <c r="J13" s="12">
         <v>1.5</v>
       </c>
@@ -1320,15 +1320,15 @@
       <c r="B14" s="12">
         <v>7</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
       <c r="J14" s="12">
         <v>3</v>
       </c>
@@ -1367,15 +1367,15 @@
       <c r="B15" s="12">
         <v>8</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12">
         <v>2.5</v>
@@ -1414,15 +1414,15 @@
       <c r="B16" s="12">
         <v>9</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12">
         <v>9</v>
@@ -1461,15 +1461,15 @@
       <c r="B17" s="12">
         <v>10</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12">
         <v>7.5</v>
@@ -1508,15 +1508,15 @@
       <c r="B18" s="12">
         <v>11</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="22"/>
       <c r="J18" s="12"/>
       <c r="K18" s="12">
         <v>0.5</v>
@@ -1557,15 +1557,15 @@
       <c r="B19" s="12">
         <v>12</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
       <c r="J19" s="12">
         <v>1.5</v>
       </c>
@@ -1612,15 +1612,15 @@
       <c r="B20" s="12">
         <v>13</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12">
@@ -1659,15 +1659,15 @@
       <c r="B21" s="12">
         <v>14</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="22"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12">
@@ -1738,7 +1738,9 @@
       <c r="P22" s="4">
         <v>0.5</v>
       </c>
-      <c r="Q22" s="4"/>
+      <c r="Q22" s="4">
+        <v>0.5</v>
+      </c>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
@@ -1754,11 +1756,11 @@
       </c>
       <c r="AC22" s="4">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="AD22" s="4">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
@@ -1786,12 +1788,18 @@
       <c r="M23" s="12">
         <v>12</v>
       </c>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
+      <c r="N23" s="4">
+        <v>1</v>
+      </c>
+      <c r="O23" s="4">
+        <v>3</v>
+      </c>
       <c r="P23" s="4">
         <v>3</v>
       </c>
-      <c r="Q23" s="4"/>
+      <c r="Q23" s="4">
+        <v>1</v>
+      </c>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
       <c r="T23" s="4"/>
@@ -1807,26 +1815,26 @@
       </c>
       <c r="AC23" s="4">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="AD23" s="4">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>17</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
@@ -1865,15 +1873,15 @@
       <c r="B25" s="12">
         <v>18</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
@@ -1912,15 +1920,15 @@
       <c r="B26" s="12">
         <v>19</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
@@ -1961,15 +1969,15 @@
       <c r="B27" s="12">
         <v>20</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
@@ -2008,15 +2016,15 @@
       <c r="B28" s="12">
         <v>21</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="22"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
@@ -2054,7 +2062,9 @@
       <c r="B29" s="4">
         <v>22</v>
       </c>
-      <c r="C29" s="17"/>
+      <c r="C29" s="17" t="s">
+        <v>52</v>
+      </c>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
@@ -2068,7 +2078,9 @@
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
+      <c r="Q29" s="4">
+        <v>11</v>
+      </c>
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
@@ -2078,25 +2090,31 @@
       <c r="X29" s="4"/>
       <c r="Y29" s="4"/>
       <c r="Z29" s="4"/>
-      <c r="AA29" s="3"/>
-      <c r="AB29" s="4"/>
+      <c r="AA29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB29" s="4">
+        <v>15</v>
+      </c>
       <c r="AC29" s="4"/>
       <c r="AD29" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <v>23</v>
       </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="44"/>
+      <c r="C30" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="19"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -2104,7 +2122,9 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
+      <c r="Q30" s="4">
+        <v>4</v>
+      </c>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
@@ -2182,11 +2202,11 @@
       </c>
       <c r="N32">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O32">
         <f t="shared" si="4"/>
-        <v>6.5</v>
+        <v>9.5</v>
       </c>
       <c r="P32">
         <f t="shared" si="4"/>
@@ -2194,7 +2214,7 @@
       </c>
       <c r="Q32">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>16.5</v>
       </c>
       <c r="R32">
         <f t="shared" si="4"/>
@@ -2238,11 +2258,11 @@
       </c>
       <c r="AC32" s="10">
         <f>SUM(AC8:AC27)</f>
-        <v>219</v>
+        <v>224.5</v>
       </c>
       <c r="AD32" s="4">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>51.5</v>
       </c>
     </row>
     <row r="33" spans="3:23" x14ac:dyDescent="0.25">

</xml_diff>